<commit_message>
añadiento archivos de prueba manual
</commit_message>
<xml_diff>
--- a/Prueba técnica.xlsx
+++ b/Prueba técnica.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linam\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linam\OneDrive\Documentos\Prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00F70F3-8719-4D2B-915C-360260BDDF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27C5A7D-8D72-4A0F-B316-1A287A74EBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9BAB7E75-803D-4FB7-87E8-244984C9FA1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Ingresar a la página www.google.com</t>
   </si>
@@ -74,29 +74,32 @@
     <t>los resultados se muestran de manera correcta junto con el tiempo que se tardó el sistema en realizar la búsqueda</t>
   </si>
   <si>
-    <t>Ingresar la palabraasccffaxadd agdccssessssaefjkk,l en la barra de búsqueda y presionar la tecla enter</t>
-  </si>
-  <si>
-    <t>Validar que no e muestren resultados  de  búsqueda</t>
-  </si>
-  <si>
-    <t>El sistema debe mostrar un mensaje: No se han encontrado resultados para tu búsqueda (asccffaxadd agdccssessssaefjkk,l).
+    <t>Validar que se muestre el botón de configuración en la esquina superior derecha dela ventana</t>
+  </si>
+  <si>
+    <t>se muestra correctamente el ícono de configuración en la ventana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dar click sobre el ícono de configuración </t>
+  </si>
+  <si>
+    <t>Al seleccionarlo se debe mostrar información asociada a la configuración rápida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la página carga correctamente </t>
+  </si>
+  <si>
+    <t>la catidad de resultados se muestran de manera correcta junto con el tiempo que se tardó el sistema en realizar la búsqueda</t>
+  </si>
+  <si>
+    <t>Ingresar la palabra asccffaxadd agdccssessssaefjkk,l en la barra de búsqueda y presionar la tecla enter</t>
+  </si>
+  <si>
+    <t>Validar que no se muestren resultados  de  búsqueda</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un mensaje que no se han encontrado datos.
 Sugerencias:</t>
-  </si>
-  <si>
-    <t>Validar que se muestre el botón de configuración en la esquina superior derecha dela ventana</t>
-  </si>
-  <si>
-    <t>se muestra correctamente el ícono de configuración en la ventana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dar click sobre el ícono de configuración </t>
-  </si>
-  <si>
-    <t>Al seleccionarlo se debe mostrar información asociada a la configuración rápida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">la página carga correctamente </t>
   </si>
 </sst>
 </file>
@@ -138,16 +141,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7027CFFC-AFBD-40BB-A6B3-48C7DBB8C80D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,16 +481,16 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -495,11 +498,11 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -507,11 +510,11 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -519,11 +522,11 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -531,11 +534,11 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -544,22 +547,22 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -567,15 +570,15 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -587,15 +590,15 @@
     </row>
     <row r="12" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -610,40 +613,40 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -651,11 +654,11 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -663,54 +666,38 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="A10:C10"/>
@@ -727,6 +714,22 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>